<commit_message>
Update notebooks and inferences
</commit_message>
<xml_diff>
--- a/inferences/places-1701.xlsx
+++ b/inferences/places-1701.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>comment</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -479,8 +484,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Zhejiang， CHEKIANG (actuel ZHEJIANG)</t>
-        </is>
+          <t>Zhejiang 浙江， CHEKIANG (actuel ZHEJIANG)</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="3">
@@ -506,8 +514,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hangzhou, </t>
-        </is>
+          <t xml:space="preserve">Hangzhou 杭州, </t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="4">
@@ -533,8 +544,11 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 海宁</t>
-        </is>
+          <t xml:space="preserve">海宁 </t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="5">
@@ -560,8 +574,11 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jiaxing, </t>
-        </is>
+          <t xml:space="preserve">Jiaxing 嘉兴, </t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="6">
@@ -587,8 +604,11 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jinhua, </t>
-        </is>
+          <t xml:space="preserve">Jinhua 金华, </t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="7">
@@ -614,8 +634,11 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lanxi, </t>
-        </is>
+          <t xml:space="preserve">Lanxi 兰溪, </t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="8">
@@ -641,8 +664,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ningbo, </t>
-        </is>
+          <t xml:space="preserve">Ningbo 宁波, </t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="9">
@@ -668,8 +694,11 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yinzhou, 鄞州 </t>
-        </is>
+          <t xml:space="preserve">Yinzhou 鄞州, </t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="10">
@@ -691,8 +720,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fujian, </t>
-        </is>
+          <t xml:space="preserve">Fujian 福建, </t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="11">
@@ -718,8 +750,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fuzhou, </t>
-        </is>
+          <t xml:space="preserve">Fuzhou 福州, </t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="12">
@@ -745,8 +780,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lianjiang, </t>
-        </is>
+          <t xml:space="preserve">Lianjiang 连江, </t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="13">
@@ -772,8 +810,11 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Zhangzhou, </t>
-        </is>
+          <t xml:space="preserve">Zhangzhou 漳州, </t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="14">
@@ -799,8 +840,11 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Quanzhou, </t>
-        </is>
+          <t xml:space="preserve">Quanzhou 泉州, </t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="15">
@@ -826,8 +870,11 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Xiamen, </t>
-        </is>
+          <t xml:space="preserve">Xiamen 厦门, </t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="16">
@@ -853,8 +900,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">(alors tcheou indépendant)Funing, </t>
-        </is>
+          <t>(alors tcheou indépendant)Funing, , hoje Xiapu 霞浦</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="17">
@@ -880,8 +930,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fu'an, </t>
-        </is>
+          <t xml:space="preserve">Fu'an 福安, </t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="18">
@@ -907,8 +960,11 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Xinghua, </t>
-        </is>
+          <t>Xinghua 兴化, , 兴化县，the wikidata code of it dose not contain coordinate information, which can be substituted by Q68579，the present-day Putian 莆田</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="19">
@@ -934,8 +990,11 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kienning fou, Jianning, </t>
-        </is>
+          <t>Kienning fou, Jianning 建寧,  the wikidata code of it does not contain coordinate information, which can be substituted by Kien-yang today Jianyang Q639862 see 1644</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="20">
@@ -964,6 +1023,9 @@
           <t xml:space="preserve">浦城 </t>
         </is>
       </c>
+      <c r="F20" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -988,8 +1050,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shaowu, </t>
-        </is>
+          <t xml:space="preserve">Shaowu 邵武, </t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="22">
@@ -1015,8 +1080,11 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jianning Xian, </t>
-        </is>
+          <t xml:space="preserve">Jianning Xian 建宁, </t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="23">
@@ -1042,8 +1110,11 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tingzhou, </t>
-        </is>
+          <t xml:space="preserve">Tingzhou 汀州, </t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="24">
@@ -1072,6 +1143,9 @@
           <t xml:space="preserve">上杭 </t>
         </is>
       </c>
+      <c r="F24" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1096,8 +1170,11 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yanping, </t>
-        </is>
+          <t xml:space="preserve">Yanping 上杭, </t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="26">
@@ -1123,8 +1200,11 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Jiangle 将乐</t>
-        </is>
+          <t xml:space="preserve">Jiangle 将乐, </t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="27">
@@ -1146,8 +1226,11 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Henan, </t>
-        </is>
+          <t xml:space="preserve">Henan 河南, </t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="28">
@@ -1173,8 +1256,11 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kaifeng, </t>
-        </is>
+          <t xml:space="preserve">Kaifeng 开封, </t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="29">
@@ -1200,8 +1286,11 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guide, </t>
-        </is>
+          <t>Guide, , hoje Shangqiu 商丘</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="30">
@@ -1223,8 +1312,11 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>(actuel HUNAN + HUBEI)Huguang</t>
-        </is>
+          <t>湖广, (actuel HUNAN + HUBEI)Huguang</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="31">
@@ -1250,8 +1342,11 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wuchang, </t>
-        </is>
+          <t xml:space="preserve">Wuchang 武昌, </t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="32">
@@ -1277,8 +1372,11 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Anlu, </t>
-        </is>
+          <t xml:space="preserve">Anlu 安陆, </t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="33">
@@ -1304,8 +1402,11 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 长沙</t>
-        </is>
+          <t xml:space="preserve">长沙 </t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="34">
@@ -1331,8 +1432,11 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Xiangtan,湘潭</t>
-        </is>
+          <t xml:space="preserve">Xiangtan 湘潭, </t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="35">
@@ -1358,8 +1462,11 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Chenzhou，郴州 Chen(g)chow</t>
-        </is>
+          <t>Chenzhou 郴州, Chen(g)chow</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="36">
@@ -1385,8 +1492,11 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>, Hengyang</t>
-        </is>
+          <t xml:space="preserve">Hengyang 衡阳, </t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="37">
@@ -1412,8 +1522,11 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jingzhou, </t>
-        </is>
+          <t xml:space="preserve">Jingzhou 荆州, </t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="38">
@@ -1442,6 +1555,9 @@
           <t>No Wikidata</t>
         </is>
       </c>
+      <c r="F38" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1466,8 +1582,11 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yongzhou, </t>
-        </is>
+          <t xml:space="preserve">Yongzhou 永州, </t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="40">
@@ -1489,8 +1608,11 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">KIANGNAN ou NANKIN (actuel ANHUI + JIANGSU),Jiangnan, </t>
-        </is>
+          <t xml:space="preserve">KIANGNAN ou NANKIN (actuel ANHUI + JIANGSU),Jiangnan 江南, </t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="41">
@@ -1516,8 +1638,11 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanjing, </t>
-        </is>
+          <t xml:space="preserve">Nanjing 南京, </t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="42">
@@ -1538,13 +1663,16 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>No wikidata</t>
+          <t>Q360374</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>wikidata:Q360374,Anqing, 安庆</t>
-        </is>
+          <t xml:space="preserve">Anqing 安庆, </t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="43">
@@ -1570,8 +1698,11 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Changzhou, </t>
-        </is>
+          <t xml:space="preserve">Changzhou 常州, </t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="44">
@@ -1597,8 +1728,11 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wuxi, 无锡, </t>
-        </is>
+          <t xml:space="preserve">Wuxi 无锡, </t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="45">
@@ -1624,8 +1758,11 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Chizhou, 池州Chinchow (= Kweichih)</t>
-        </is>
+          <t>Chizhou 池州, Chinchow (= Kweichih)</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="46">
@@ -1651,8 +1788,11 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Zhenjiang, </t>
-        </is>
+          <t xml:space="preserve">Zhenjiang 镇江, </t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="47">
@@ -1678,8 +1818,11 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Danyang, </t>
-        </is>
+          <t xml:space="preserve">Danyang 丹阳, </t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="48">
@@ -1705,8 +1848,11 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 凤阳</t>
-        </is>
+          <t xml:space="preserve">凤阳, </t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="49">
@@ -1732,8 +1878,11 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>.Wuhe, 五河</t>
-        </is>
+          <t xml:space="preserve">Wuhe 五河, </t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="50">
@@ -1759,8 +1908,11 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Huai'an, </t>
-        </is>
+          <t xml:space="preserve">Huai'an 淮安, </t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="51">
@@ -1781,13 +1933,16 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Q57719</t>
+          <t>Q42622</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Xuzhou, 徐州</t>
-        </is>
+          <t xml:space="preserve">Suzhou 苏州, </t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="52">
@@ -1813,8 +1968,11 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Changshu (Cham xo), Changshu, </t>
-        </is>
+          <t xml:space="preserve">Changshu (Cham xo), Changshu 常熟, </t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="53">
@@ -1840,8 +1998,11 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>,Kunshan, 昆山</t>
-        </is>
+          <t xml:space="preserve">昆山, </t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="54">
@@ -1862,13 +2023,16 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Q42622</t>
+          <t>Q57719</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Suzhou, </t>
-        </is>
+          <t xml:space="preserve">Xuzhou 徐州, </t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="55">
@@ -1894,8 +2058,11 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Songjiang, </t>
-        </is>
+          <t xml:space="preserve">Songjiang 松江, </t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="56">
@@ -1921,8 +2088,11 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shanghai, </t>
-        </is>
+          <t xml:space="preserve">Shanghai 上海, </t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="57">
@@ -1951,6 +2121,9 @@
           <t xml:space="preserve">Qingpu, </t>
         </is>
       </c>
+      <c r="F57" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1975,8 +2148,11 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Taicang, 太仓</t>
-        </is>
+          <t xml:space="preserve">Taicang 太仓, </t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="59">
@@ -2002,8 +2178,11 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jiading, </t>
-        </is>
+          <t xml:space="preserve">Jiading 嘉定, </t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="60">
@@ -2029,8 +2208,11 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chongming, </t>
-        </is>
+          <t xml:space="preserve">Chongming 崇明, </t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="61">
@@ -2056,8 +2238,11 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yangzhou, </t>
-        </is>
+          <t xml:space="preserve">Yangzhou 扬州, </t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="62">
@@ -2079,8 +2264,11 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jiangxi, </t>
-        </is>
+          <t xml:space="preserve">Jiangxi 江西, </t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="63">
@@ -2106,8 +2294,11 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanchang, </t>
-        </is>
+          <t xml:space="preserve">Nanchang 南昌, </t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="64">
@@ -2133,8 +2324,11 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>, Fuzhou, 抚州</t>
-        </is>
+          <t xml:space="preserve">Fuzhou 抚州, </t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="65">
@@ -2160,8 +2354,11 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Raozhou, 饶州,present day Poyang County</t>
-        </is>
+          <t>Raozhou 饶州, , present day Poyang County</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="66">
@@ -2190,6 +2387,9 @@
           <t xml:space="preserve">Ganzhou (赣州) in Jiangxi </t>
         </is>
       </c>
+      <c r="F66" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2214,8 +2414,11 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>,Ningdu, 宁都</t>
-        </is>
+          <t xml:space="preserve">Ningdu 宁都, </t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="68">
@@ -2241,8 +2444,11 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>, Xinfeng,信丰</t>
-        </is>
+          <t xml:space="preserve">Xinfeng 信丰, </t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="69">
@@ -2268,8 +2474,11 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>,Ji'an,吉安</t>
-        </is>
+          <t xml:space="preserve">Ji'an 吉安, </t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="70">
@@ -2295,8 +2504,11 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>, Dingnan, 定南</t>
-        </is>
+          <t xml:space="preserve">Dingnan 定南, </t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="71">
@@ -2322,8 +2534,11 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jianchang, </t>
-        </is>
+          <t xml:space="preserve">Jianchang 建昌, </t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="72">
@@ -2349,8 +2564,11 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanfeng, </t>
-        </is>
+          <t xml:space="preserve">Nanfeng 南丰, </t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="73">
@@ -2376,8 +2594,11 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>,Jiujiang, 九江</t>
-        </is>
+          <t xml:space="preserve">Jiujiang 九江, </t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="74">
@@ -2403,8 +2624,11 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Guangxin, 广信</t>
-        </is>
+          <t xml:space="preserve">Guangxin 广信, </t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="75">
@@ -2430,8 +2654,11 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>,Yushan, 玉山</t>
-        </is>
+          <t xml:space="preserve">玉山, </t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="76">
@@ -2457,8 +2684,11 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nan'an, </t>
-        </is>
+          <t xml:space="preserve">Nan'an 南安, </t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="77">
@@ -2487,6 +2717,9 @@
           <t>No wikidata</t>
         </is>
       </c>
+      <c r="F77" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2507,8 +2740,11 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guangxi, </t>
-        </is>
+          <t xml:space="preserve">Guangxi 广西, </t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="79">
@@ -2534,8 +2770,11 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guilin, </t>
-        </is>
+          <t xml:space="preserve">Guilin 桂林, </t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="80">
@@ -2561,8 +2800,11 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wuzhou, </t>
-        </is>
+          <t xml:space="preserve">Wuzhou 梧州, </t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="81">
@@ -2584,8 +2826,11 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guangdong, </t>
-        </is>
+          <t xml:space="preserve">Guangdong 广东, </t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="82">
@@ -2611,8 +2856,11 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>,Guangzhou, 广州Canton</t>
-        </is>
+          <t>Guangzhou 广州, Canton</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="83">
@@ -2638,8 +2886,11 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>,Foshan, 佛山</t>
-        </is>
+          <t xml:space="preserve">Foshan 佛山, </t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="84">
@@ -2660,13 +2911,16 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>No wikidata</t>
+          <t>Q1023903</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>wikidata:Q1023903,Xinhui, 新会</t>
-        </is>
+          <t xml:space="preserve">Xinhui 新会, </t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="85">
@@ -2692,8 +2946,11 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dongguan, </t>
-        </is>
+          <t xml:space="preserve">Dongguan 东莞, </t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="86">
@@ -2719,8 +2976,11 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kiungchow (île de Hainan), Qiongzhou, </t>
-        </is>
+          <t>琼州, Kiungchow (île de Hainan), Qiongzhou</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="87">
@@ -2746,8 +3006,11 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>, Lianzhou, 廉州 present day Hepu County</t>
-        </is>
+          <t>Lianzhou 廉州, , present day Hepu County</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="88">
@@ -2773,8 +3036,11 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leizhou, </t>
-        </is>
+          <t xml:space="preserve">Leizhou 雷州, </t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="89">
@@ -2800,8 +3066,11 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanxiong, </t>
-        </is>
+          <t xml:space="preserve">Nanxiong 南雄, </t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="90">
@@ -2827,8 +3096,11 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Shixing, 始兴</t>
-        </is>
+          <t xml:space="preserve">Shixing 始兴, </t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="91">
@@ -2854,8 +3126,11 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>,Shuntak (Xunte Shunde, 顺德Shuntak (Xunte)</t>
-        </is>
+          <t xml:space="preserve">Xunte Shunde 顺德, </t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="92">
@@ -2884,6 +3159,9 @@
           <t>No wikidataShiuhow (Xao cheu)</t>
         </is>
       </c>
+      <c r="F92" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2908,8 +3186,11 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>,Lecong, 乐从</t>
-        </is>
+          <t xml:space="preserve">Lecong 乐从, </t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="94">
@@ -2938,6 +3219,9 @@
           <t>No wikidataYanfa -- Gin hoa</t>
         </is>
       </c>
+      <c r="F94" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2962,8 +3246,11 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chao Kim, Zhaoqing, </t>
-        </is>
+          <t xml:space="preserve">Chao Kim, Zhaoqing 肇庆, </t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="96">
@@ -2989,8 +3276,11 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>,Huizhou,惠州Waichow, Hwaichow (Hoei cheu), Guizhou,</t>
-        </is>
+          <t>Huizhou,惠州 Waichow, Hwaichow (Hoei cheu), Guizhou,</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="97">
@@ -3015,6 +3305,9 @@
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
+      <c r="F97" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3042,6 +3335,9 @@
           <t xml:space="preserve">Ilha Verde, </t>
         </is>
       </c>
+      <c r="F98" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3069,6 +3365,9 @@
           <t xml:space="preserve">Lapa (Wan-tchai),Wanzai, </t>
         </is>
       </c>
+      <c r="F99" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3089,8 +3388,11 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t xml:space="preserve">KWEICHOW (actuel GUIZHOU): néant Guizhou, </t>
-        </is>
+          <t xml:space="preserve">KWEICHOW (actuel GUIZHOU): néant Guizhou 贵州, </t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="101">
@@ -3112,8 +3414,11 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>PEKING (actuel HEBEI)</t>
-        </is>
+          <t>PEKING (actuel HEBEI) 北京</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="102">
@@ -3139,8 +3444,11 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pékin collège St Joseph (1605) ou Si-t'ang (sera appelé Nan-t'ang en 1723, à cause du Si-t'ang fondé pour la Propagande, R), Beijing, </t>
-        </is>
+          <t>Beijing 北京, Pékin collège St Joseph (1605) ou Si-t'ang (sera appelé Nan-t'ang en 1723, à cause du Si-t'ang fondé pour la Propagande, R)</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="103">
@@ -3166,8 +3474,11 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 西堂Si-t'ang fondé pour la Propagande, R [em 1703])</t>
-        </is>
+          <t>Xitang 西堂  西堂Si-t'ang fondé pour la Propagande, R [em 1703])</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="104">
@@ -3193,8 +3504,11 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 东堂Tong-t'ang ou R Saint-Joseph (1655)</t>
-        </is>
+          <t>Dongtang 东堂  东堂Tong-t'ang ou R Saint-Joseph (1655)</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="105">
@@ -3220,8 +3534,11 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 北堂</t>
-        </is>
+          <t xml:space="preserve">Beitang, 北堂 </t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="106">
@@ -3247,8 +3564,11 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Liangxiang, 良乡</t>
-        </is>
+          <t xml:space="preserve">Liangxiang 良乡, </t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="107">
@@ -3274,8 +3594,11 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tongzhou, </t>
-        </is>
+          <t xml:space="preserve">Tongzhou 通州, </t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="108">
@@ -3301,8 +3624,11 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Zhengding, </t>
-        </is>
+          <t xml:space="preserve">Zhengding 正定, </t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="109">
@@ -3328,8 +3654,11 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Baoding, </t>
-        </is>
+          <t xml:space="preserve">Baoding 保定, </t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="110">
@@ -3351,8 +3680,11 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shanxi, </t>
-        </is>
+          <t xml:space="preserve">Shanxi 山西, </t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="111">
@@ -3378,8 +3710,11 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">Taiyuan, </t>
-        </is>
+          <t xml:space="preserve">Taiyuan 太原, </t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="112">
@@ -3405,8 +3740,11 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>,Fenzhou, 汾州</t>
-        </is>
+          <t xml:space="preserve">Fenzhou 汾州, </t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="113">
@@ -3432,8 +3770,11 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>, 平遥Pingyao du Fenchow</t>
-        </is>
+          <t xml:space="preserve">Pingyao du Fenchow 平遥, </t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="114">
@@ -3459,8 +3800,11 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Jiexiu, 介休Kiehsiu du Fenchow</t>
-        </is>
+          <t>Jiexiu 介休, Kiehsiu du Fenchow</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="115">
@@ -3489,6 +3833,9 @@
           <t>Pingyang Fu, , Q73156</t>
         </is>
       </c>
+      <c r="F115" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3516,6 +3863,9 @@
           <t xml:space="preserve">Jiangzhou, </t>
         </is>
       </c>
+      <c r="F116" t="n">
+        <v>1701</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3540,8 +3890,11 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Puzhou, </t>
-        </is>
+          <t xml:space="preserve">Puzhou 绛州, </t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="118">
@@ -3562,13 +3915,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Q1197616</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 洪洞</t>
-        </is>
+          <t>No wikidata</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="119">
@@ -3584,18 +3936,21 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Kiehsiu</t>
+          <t>Siangling</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Q1362530</t>
+          <t>Q22099543</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Jiexiu, 介休</t>
-        </is>
+          <t xml:space="preserve">Xiangling 襄陵县，the wikidata code of it does not contain coordination information, which can be substituted by Q1197358，present day Xiangfen County 襄汾县, </t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="120">
@@ -3611,18 +3966,21 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Siangling</t>
+          <t>Taiping</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Q22099543</t>
+          <t>Q18111423</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Xiangling 襄陵县，the wikidata code of it dose not contain coordination information, which can be substituted by Q1197358，present day Xiangfen County 襄汾县</t>
-        </is>
+          <t>Taiping 太平县，the wikidata code of it does not contain coordinate information, which can be substituted by Q11137509，the present-day 汾城镇 , , Q1113750</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="121">
@@ -3638,18 +3996,21 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Taiping</t>
+          <t>Wanchuan</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Q18111423</t>
+          <t>Q8475332</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Taiping, ,太平县，the wikidata code of it dose not contain coordinate information, which can be substituted by Q11137509，the present-day 汾城镇</t>
-        </is>
+          <t xml:space="preserve">Wanquan 万泉县，the wikidata code of it does not contain coordinate information, which can be substituted by Q1196908，the present-day万荣县, </t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="122">
@@ -3660,23 +4021,26 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Pingyang</t>
+          <t>Sinchow</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Wanchuan</t>
+          <t>Sinchow</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Q8475332</t>
+          <t>Q73119</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 万泉县，the wikidata code of it dose not contain coordinate information, which can be substituted by Q1196908，the present-day万荣县</t>
-        </is>
+          <t xml:space="preserve">Xinzhou 忻州, </t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="123">
@@ -3692,45 +4056,47 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Sinchow</t>
+          <t>Tsinglo</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Q73119</t>
+          <t>Q174034</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>,Xinzhou, 忻州</t>
-        </is>
+          <t xml:space="preserve">Jingle 静乐, </t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Shansi</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>Sinchow</t>
-        </is>
-      </c>
+          <t>Shantung</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr"/>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Tsinglo</t>
+          <t>Shantung</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Q174034</t>
+          <t>Q43407</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>,Jingle, 静乐</t>
-        </is>
+          <t xml:space="preserve">actuel Shandong, Shandong 山东, </t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="125">
@@ -3739,21 +4105,28 @@
           <t>Shantung</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Tsinan</t>
+        </is>
+      </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Shantung</t>
+          <t>Tsinan</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Q43407</t>
+          <t>Q170247</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t xml:space="preserve">actuel Shandong, Shandong, </t>
-        </is>
+          <t xml:space="preserve">Jinan 济南, </t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="126">
@@ -3769,18 +4142,21 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Tsinan</t>
+          <t>Taian</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Q170247</t>
+          <t>Q217681</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jinan, </t>
-        </is>
+          <t xml:space="preserve">Tai'an 泰安, </t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="127">
@@ -3796,18 +4172,21 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Taian</t>
+          <t>Tehchow</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Q217681</t>
+          <t>Q162880</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tai'an, </t>
-        </is>
+          <t xml:space="preserve">Dezhou 德州, </t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="128">
@@ -3818,23 +4197,26 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Tsinan</t>
+          <t>Tsingchow</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Tehchow</t>
+          <t>Tsingchow</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Q162880</t>
+          <t>Q1360781</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>,Dezhou,德州</t>
-        </is>
+          <t xml:space="preserve">(-- Idu, Yitu)Qingzhou 青州, , Yidu, </t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="129">
@@ -3845,23 +4227,26 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Tsingchow</t>
+          <t>Linchu</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Tsingchow</t>
+          <t>Linchu</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Q1360781</t>
+          <t>Q1198208</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t xml:space="preserve">(-- Idu, Yitu)Qingzhou, , Yidu, </t>
-        </is>
+          <t xml:space="preserve">Linkiu 临朐, </t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="130">
@@ -3872,23 +4257,26 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Linchu</t>
+          <t>Tungchang</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Linchu</t>
+          <t>Tungchang</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Q1198208</t>
+          <t>Q10870440</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>,Linkiu, 临朐</t>
-        </is>
+          <t xml:space="preserve">Dungchang 东昌, </t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="131">
@@ -3904,18 +4292,21 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Tungchang</t>
+          <t>Lintsing</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Q10870440</t>
+          <t>Q1207099</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dungchang, </t>
-        </is>
+          <t xml:space="preserve">Linqing 临清, </t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="132">
@@ -3926,23 +4317,26 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Tungchang</t>
+          <t>Yenchow</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Lintsing</t>
+          <t>Yenchow</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>No wikidata</t>
+          <t>Q10891140</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>wikidata:Q1207099.Linqing, 临清</t>
-        </is>
+          <t xml:space="preserve">Yanzhou 兖州, </t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="133">
@@ -3958,18 +4352,21 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Yenchow</t>
+          <t>Ichow</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Q10891140</t>
+          <t>Q11552388</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Yanzhou, 兖州</t>
-        </is>
+          <t>(hoje Linyi, Shandong) 沂州, Ichow (-- Lini), alors tcheou</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="134">
@@ -3985,45 +4382,47 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Ichow</t>
+          <t>Tsining</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Q11552388</t>
+          <t>Q372791</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Ichow ( -- Lini)</t>
-        </is>
+          <t xml:space="preserve">Jining 济宁, </t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Shantung</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Yenchow</t>
-        </is>
-      </c>
+          <t>Shensi</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr"/>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Tsining</t>
+          <t>Shensi</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Q372791</t>
+          <t>Q46913</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>,Jining, 济宁</t>
-        </is>
+          <t>Hoje Shaanxi para distinguir de deh-r1701-shansi (actuel SHANXI)Shanxi</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="136">
@@ -4032,21 +4431,28 @@
           <t>Shensi</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Sian</t>
+        </is>
+      </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Shensi</t>
+          <t>Sian</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Q46913</t>
+          <t>Q5826</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>(actuel SHANXI)Shanxi,  Shaanxi 陕西</t>
-        </is>
+          <t xml:space="preserve">Xi'an 西安, </t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="137">
@@ -4062,18 +4468,21 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Sian</t>
+          <t>Sanyuan</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Q5826</t>
+          <t>Q1201362</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Xi'an, </t>
-        </is>
+          <t xml:space="preserve">Sanyuan 三原, </t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="138">
@@ -4084,23 +4493,26 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Sian</t>
+          <t>Hanchung</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Sanyuan</t>
+          <t>Hanchung</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Q1201362</t>
+          <t>Q515573</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sanyuan, </t>
-        </is>
+          <t xml:space="preserve">Hanzhong 汉中, </t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="139">
@@ -4111,23 +4523,26 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Hanchung</t>
+          <t>Chengku</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Hanchung</t>
+          <t>Chengku</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Q515573</t>
+          <t>Q1069968</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hanzhong, </t>
-        </is>
+          <t xml:space="preserve">Chenggu 城固, </t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="140">
@@ -4143,45 +4558,47 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Chengku</t>
+          <t>Siao-tchai</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Q1069968</t>
+          <t>No wikidata</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chenggu, </t>
-        </is>
+          <t>No wikidataSiao-tchai du Chengku</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Shensi</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Chengku</t>
-        </is>
-      </c>
+          <t>Szechwan</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr"/>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Siao-tchai</t>
+          <t>Szechwan</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>No wikidata</t>
+          <t>Q19770</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>No wikidataSiao-tchai du Chengku</t>
-        </is>
+          <t xml:space="preserve">actuel SICHUAN)Sichuan 四川, </t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="142">
@@ -4190,21 +4607,28 @@
           <t>Szechwan</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr"/>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Chengtu</t>
+        </is>
+      </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Szechwan</t>
+          <t>Chengtu</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Q19770</t>
+          <t>Q30002</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t xml:space="preserve">actuel SICHUAN)Sichuan, </t>
-        </is>
+          <t xml:space="preserve">Chengdu 成都, </t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="143">
@@ -4215,50 +4639,52 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Chengtu</t>
+          <t>Chungking</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Chengtu</t>
+          <t>Chungking</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Q30002</t>
+          <t>Q11725</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chengdu, </t>
-        </is>
+          <t xml:space="preserve">Chongqing 重庆, </t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Szechwan</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>Chungking</t>
-        </is>
-      </c>
+          <t>Yunnan</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr"/>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Chungking</t>
+          <t>Yunnan</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Q11725</t>
+          <t>Q43194</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chongqing, </t>
-        </is>
+          <t xml:space="preserve">Yunnan 云南, </t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>1701</v>
       </c>
     </row>
     <row r="145">
@@ -4267,45 +4693,29 @@
           <t>Yunnan</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr"/>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Yunnanfu</t>
+        </is>
+      </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Yunnan</t>
+          <t>Yunnanfu</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Q43194</t>
+          <t>Q182852</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yunnan, </t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Yunnan</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>Yunnanfu</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Yunnanfu</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>No wikidata</t>
-        </is>
-      </c>
-      <c r="E146" t="inlineStr"/>
+          <t xml:space="preserve">Yunanfu,present day Kunming 昆明, </t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>1701</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>